<commit_message>
Conversion Excel vers SKOS
</commit_message>
<xml_diff>
--- a/fr.sparna/rdf/skos/xls2skos/src/test/resources/testExcelNative.xlsx
+++ b/fr.sparna/rdf/skos/xls2skos/src/test/resources/testExcelNative.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>http://data.sparna.fr/scheme/days</t>
   </si>
@@ -33,9 +33,6 @@
     <t>The days of the week</t>
   </si>
   <si>
-    <t>This is a general comment that will be ignored. The converter will detect automatically the ligne containing the column titles below, so you can have a ConceptScheme as long as you want.</t>
-  </si>
-  <si>
     <t>URI</t>
   </si>
   <si>
@@ -139,13 +136,49 @@
   </si>
   <si>
     <t>WKND</t>
+  </si>
+  <si>
+    <t>PREFIX</t>
+  </si>
+  <si>
+    <t>euvoc</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/ontology/euvoc#</t>
+  </si>
+  <si>
+    <t>euvoc:status</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/concept-status/CURRENT</t>
+  </si>
+  <si>
+    <t>http://publications.europa.eu/resource/authority/concept-status/TESTING</t>
+  </si>
+  <si>
+    <t>This is a general comment that will be ignored. The converter will detect automatically the line containing the column titles below, so you can have a header as long as you want.</t>
+  </si>
+  <si>
+    <t>euvoc:comment</t>
+  </si>
+  <si>
+    <t>Check with Andrew if the concept of Week-end is the same in the US, in China and the UK. Try to determine a universal notion of what a "week-end" is.</t>
+  </si>
+  <si>
+    <t>Note that some consider Sunday to be the first day of the week. Should we give ordering numbers to weekdays ?</t>
+  </si>
+  <si>
+    <t>rdf:type</t>
+  </si>
+  <si>
+    <t>http://data.sparna.fr/ontology/day</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,13 +186,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -171,17 +225,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -486,171 +553,236 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="69.85546875" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="B8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="30">
-      <c r="A8" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="30">
-      <c r="A9" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="F10" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F11" t="s">
         <v>20</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
+      <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="F13" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
+      <c r="C14" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F14" t="s">
         <v>30</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="60">
+      <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" t="s">
         <v>32</v>
       </c>
-      <c r="B14" t="s">
+      <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="F15" t="s">
         <v>34</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="77.25" customHeight="1">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="60">
-      <c r="A15" t="s">
+      <c r="B16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="E15" t="s">
-        <v>40</v>
+      <c r="G16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G16" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>